<commit_message>
updating the code of final project
</commit_message>
<xml_diff>
--- a/Inditex_Simplified_ModelB - Copy.xlsx
+++ b/Inditex_Simplified_ModelB - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadir\Desktop\BAAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E5E14C-9554-4218-92EA-6D71D16B16B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244D4493-4AE0-4509-B333-85951CDBB8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>